<commit_message>
Score generator geliştirildi. Kod refactor edildi. Query Facade patterninde tekrar yazıldı.
</commit_message>
<xml_diff>
--- a/scores/2025-04-07.xlsx
+++ b/scores/2025-04-07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arcelik-my.sharepoint.com/personal/ar002288_arcelik_com/Documents/Academy/Lecture Notes/HBM596E/Exploration/SemanticKernel/scores/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_486DD1B8D3B0DB2443383311595ED87656CDA883" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA98C79C-6E38-47E2-842E-57DEE6C4A7C5}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_486DD1B8D3B0DB2443383311595ED87656CDA883" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD89C557-06FD-41EE-AA2D-AE9EB47270C0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,13 +18,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="43">
   <si>
     <t>Answer Model</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Average of Avg Score</t>
+  </si>
+  <si>
+    <t>Count of Question #</t>
   </si>
 </sst>
 </file>
@@ -1180,10 +1183,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FA10CE84-7620-4B7F-8928-DD93E9C41A69}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
-  <location ref="A3:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FA10CE84-7620-4B7F-8928-DD93E9C41A69}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" multipleFieldFilters="0">
+  <location ref="A3:E9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
       <items count="6">
         <item x="0"/>
         <item x="1"/>
@@ -1192,9 +1195,18 @@
         <item x="4"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1205,19 +1217,19 @@
   </rowFields>
   <rowItems count="6">
     <i>
-      <x/>
-    </i>
-    <i>
       <x v="1"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x/>
     </i>
     <i>
       <x v="3"/>
     </i>
     <i>
-      <x v="4"/>
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -1226,7 +1238,7 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="4">
     <i>
       <x/>
     </i>
@@ -1236,11 +1248,15 @@
     <i i="2">
       <x v="2"/>
     </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
   </colItems>
-  <dataFields count="3">
+  <dataFields count="4">
     <dataField name="Average of SQL (Data Result)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Average of Python (Visualization)" fld="4" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Average of Avg Score" fld="5" subtotal="average" baseField="0" baseItem="1"/>
+    <dataField name="Count of Question #" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1539,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479BAA5E-8CF9-4903-A789-A6A2EE889790}">
-  <dimension ref="A3:D9"/>
+  <dimension ref="A3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,9 +1567,10 @@
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -1566,50 +1583,62 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4">
+        <v>98.75</v>
+      </c>
+      <c r="C4" s="4">
+        <v>77.5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>88.125</v>
+      </c>
+      <c r="E4" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4">
+        <v>92.5</v>
+      </c>
+      <c r="C5" s="4">
+        <v>67.5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>80</v>
+      </c>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>97.5</v>
-      </c>
-      <c r="C4" s="4">
-        <v>51.25</v>
-      </c>
-      <c r="D4" s="4">
-        <v>74.375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="4">
-        <v>98.75</v>
-      </c>
-      <c r="C5" s="4">
-        <v>77.5</v>
-      </c>
-      <c r="D5" s="4">
-        <v>88.125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="B6" s="4">
         <v>97.5</v>
       </c>
       <c r="C6" s="4">
-        <v>35</v>
+        <v>51.25</v>
       </c>
       <c r="D6" s="4">
-        <v>66.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74.375</v>
+      </c>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1622,22 +1651,28 @@
       <c r="D7" s="4">
         <v>71.875</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="4">
-        <v>92.5</v>
+        <v>97.5</v>
       </c>
       <c r="C8" s="4">
-        <v>67.5</v>
+        <v>35</v>
       </c>
       <c r="D8" s="4">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66.25</v>
+      </c>
+      <c r="E8" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
@@ -1649,6 +1684,9 @@
       </c>
       <c r="D9" s="4">
         <v>76.125</v>
+      </c>
+      <c r="E9" s="4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>